<commit_message>
Fixed bug in saving function
</commit_message>
<xml_diff>
--- a/Grids_and_profiles/grids/IEEE 14.xlsx
+++ b/Grids_and_profiles/grids/IEEE 14.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spenate\Desktop\GitHub\GridCal\Grids_and_profiles\grids\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="708" firstSheet="6" activeTab="10"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -27,12 +22,12 @@
     <sheet name="shunt" sheetId="13" r:id="rId13"/>
     <sheet name="shunt_Y_profiles" sheetId="14" r:id="rId14"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="167">
   <si>
     <t>Property</t>
   </si>
@@ -181,88 +176,88 @@
     <t>0j</t>
   </si>
   <si>
-    <t>-2246.0</t>
-  </si>
-  <si>
-    <t>-1993.0</t>
-  </si>
-  <si>
-    <t>-1776.0</t>
-  </si>
-  <si>
-    <t>-1874.0</t>
-  </si>
-  <si>
-    <t>-2217.0</t>
-  </si>
-  <si>
-    <t>-2891.0</t>
-  </si>
-  <si>
-    <t>-1916.0</t>
-  </si>
-  <si>
-    <t>-1802.0</t>
-  </si>
-  <si>
-    <t>-2181.0</t>
-  </si>
-  <si>
-    <t>-2450.0</t>
-  </si>
-  <si>
-    <t>-2649.0</t>
-  </si>
-  <si>
-    <t>-3507.0</t>
-  </si>
-  <si>
-    <t>-3097.0</t>
-  </si>
-  <si>
-    <t>-2701.0</t>
-  </si>
-  <si>
-    <t>-549.0</t>
-  </si>
-  <si>
-    <t>-648.0</t>
-  </si>
-  <si>
-    <t>-659.0</t>
-  </si>
-  <si>
-    <t>-1016.0</t>
-  </si>
-  <si>
-    <t>-795.0</t>
-  </si>
-  <si>
-    <t>-722.0</t>
-  </si>
-  <si>
-    <t>-1291.0</t>
-  </si>
-  <si>
-    <t>-1563.0</t>
-  </si>
-  <si>
-    <t>-1248.0</t>
-  </si>
-  <si>
-    <t>-1192.0</t>
-  </si>
-  <si>
-    <t>-1044.0</t>
-  </si>
-  <si>
-    <t>-1112.0</t>
-  </si>
-  <si>
-    <t>-1290.0</t>
-  </si>
-  <si>
-    <t>-1446.0</t>
+    <t>-3102.0</t>
+  </si>
+  <si>
+    <t>-2849.0</t>
+  </si>
+  <si>
+    <t>-2632.0</t>
+  </si>
+  <si>
+    <t>-2730.0</t>
+  </si>
+  <si>
+    <t>-3073.0</t>
+  </si>
+  <si>
+    <t>-3747.0</t>
+  </si>
+  <si>
+    <t>-2772.0</t>
+  </si>
+  <si>
+    <t>-2658.0</t>
+  </si>
+  <si>
+    <t>-3037.0</t>
+  </si>
+  <si>
+    <t>-3306.0</t>
+  </si>
+  <si>
+    <t>-3505.0</t>
+  </si>
+  <si>
+    <t>-4363.0</t>
+  </si>
+  <si>
+    <t>-3953.0</t>
+  </si>
+  <si>
+    <t>-3557.0</t>
+  </si>
+  <si>
+    <t>-1069.0</t>
+  </si>
+  <si>
+    <t>-1168.0</t>
+  </si>
+  <si>
+    <t>-1179.0</t>
+  </si>
+  <si>
+    <t>-1536.0</t>
+  </si>
+  <si>
+    <t>-1315.0</t>
+  </si>
+  <si>
+    <t>-1242.0</t>
+  </si>
+  <si>
+    <t>-1811.0</t>
+  </si>
+  <si>
+    <t>-2083.0</t>
+  </si>
+  <si>
+    <t>-1768.0</t>
+  </si>
+  <si>
+    <t>-1712.0</t>
+  </si>
+  <si>
+    <t>-1564.0</t>
+  </si>
+  <si>
+    <t>-1632.0</t>
+  </si>
+  <si>
+    <t>-1810.0</t>
+  </si>
+  <si>
+    <t>-1966.0</t>
   </si>
   <si>
     <t>60.0</t>
@@ -283,7 +278,7 @@
     <t>132.97786720321938</t>
   </si>
   <si>
-    <t>114.42434664769327</t>
+    <t>114.42434664769328</t>
   </si>
   <si>
     <t>122.89035612622295</t>
@@ -298,7 +293,7 @@
     <t>120.81488933601601</t>
   </si>
   <si>
-    <t>121.68092620071864</t>
+    <t>121.68092620071863</t>
   </si>
   <si>
     <t>105.89786567288776</t>
@@ -538,11 +533,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -608,19 +603,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -662,7 +649,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -694,10 +681,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -729,7 +715,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -905,14 +890,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -920,7 +905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -931,7 +916,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -942,7 +927,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -959,16 +944,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1003,7 +986,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1041,7 +1024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1058,7 +1041,7 @@
         <v>40</v>
       </c>
       <c r="F3">
-        <v>1.0449999999999999</v>
+        <v>1.045</v>
       </c>
       <c r="G3">
         <v>9999</v>
@@ -1079,7 +1062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1117,7 +1100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1155,7 +1138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1172,7 +1155,7 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>1.0900000000000001</v>
+        <v>1.09</v>
       </c>
       <c r="G6">
         <v>9999</v>
@@ -1199,16 +1182,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="B1" s="1" t="s">
         <v>159</v>
       </c>
@@ -1225,7 +1206,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="2">
         <v>43101</v>
       </c>
@@ -1233,7 +1214,7 @@
         <v>1.06</v>
       </c>
       <c r="C2">
-        <v>1.0449999999999999</v>
+        <v>1.045</v>
       </c>
       <c r="D2">
         <v>1.01</v>
@@ -1242,18 +1223,18 @@
         <v>1.07</v>
       </c>
       <c r="F2">
-        <v>1.0900000000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.09</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="2">
-        <v>43101.041666666657</v>
+        <v>43101.04166666666</v>
       </c>
       <c r="B3">
         <v>1.06</v>
       </c>
       <c r="C3">
-        <v>1.0449999999999999</v>
+        <v>1.045</v>
       </c>
       <c r="D3">
         <v>1.01</v>
@@ -1262,18 +1243,18 @@
         <v>1.07</v>
       </c>
       <c r="F3">
-        <v>1.0900000000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.09</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="2">
-        <v>43101.083333333343</v>
+        <v>43101.08333333334</v>
       </c>
       <c r="B4">
         <v>1.06</v>
       </c>
       <c r="C4">
-        <v>1.0449999999999999</v>
+        <v>1.045</v>
       </c>
       <c r="D4">
         <v>1.01</v>
@@ -1282,10 +1263,10 @@
         <v>1.07</v>
       </c>
       <c r="F4">
-        <v>1.0900000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.09</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="2">
         <v>43101.125</v>
       </c>
@@ -1293,7 +1274,7 @@
         <v>1.06</v>
       </c>
       <c r="C5">
-        <v>1.0449999999999999</v>
+        <v>1.045</v>
       </c>
       <c r="D5">
         <v>1.01</v>
@@ -1302,18 +1283,18 @@
         <v>1.07</v>
       </c>
       <c r="F5">
-        <v>1.0900000000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.09</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="2">
-        <v>43101.166666666657</v>
+        <v>43101.16666666666</v>
       </c>
       <c r="B6">
         <v>1.06</v>
       </c>
       <c r="C6">
-        <v>1.0449999999999999</v>
+        <v>1.045</v>
       </c>
       <c r="D6">
         <v>1.01</v>
@@ -1322,18 +1303,18 @@
         <v>1.07</v>
       </c>
       <c r="F6">
-        <v>1.0900000000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.09</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="2">
-        <v>43101.208333333343</v>
+        <v>43101.20833333334</v>
       </c>
       <c r="B7">
         <v>1.06</v>
       </c>
       <c r="C7">
-        <v>1.0449999999999999</v>
+        <v>1.045</v>
       </c>
       <c r="D7">
         <v>1.01</v>
@@ -1342,10 +1323,10 @@
         <v>1.07</v>
       </c>
       <c r="F7">
-        <v>1.0900000000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.09</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="2">
         <v>43101.25</v>
       </c>
@@ -1353,7 +1334,7 @@
         <v>1.06</v>
       </c>
       <c r="C8">
-        <v>1.0449999999999999</v>
+        <v>1.045</v>
       </c>
       <c r="D8">
         <v>1.01</v>
@@ -1362,18 +1343,18 @@
         <v>1.07</v>
       </c>
       <c r="F8">
-        <v>1.0900000000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.09</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="2">
-        <v>43101.291666666657</v>
+        <v>43101.29166666666</v>
       </c>
       <c r="B9">
         <v>1.06</v>
       </c>
       <c r="C9">
-        <v>1.0449999999999999</v>
+        <v>1.045</v>
       </c>
       <c r="D9">
         <v>1.01</v>
@@ -1382,18 +1363,18 @@
         <v>1.07</v>
       </c>
       <c r="F9">
-        <v>1.0900000000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.09</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="2">
-        <v>43101.333333333343</v>
+        <v>43101.33333333334</v>
       </c>
       <c r="B10">
         <v>1.06</v>
       </c>
       <c r="C10">
-        <v>1.0449999999999999</v>
+        <v>1.045</v>
       </c>
       <c r="D10">
         <v>1.01</v>
@@ -1402,10 +1383,10 @@
         <v>1.07</v>
       </c>
       <c r="F10">
-        <v>1.0900000000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.09</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="2">
         <v>43101.375</v>
       </c>
@@ -1413,7 +1394,7 @@
         <v>1.06</v>
       </c>
       <c r="C11">
-        <v>1.0449999999999999</v>
+        <v>1.045</v>
       </c>
       <c r="D11">
         <v>1.01</v>
@@ -1422,7 +1403,7 @@
         <v>1.07</v>
       </c>
       <c r="F11">
-        <v>1.0900000000000001</v>
+        <v>1.09</v>
       </c>
     </row>
   </sheetData>
@@ -1431,16 +1412,14 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="B1" s="1" t="s">
         <v>159</v>
       </c>
@@ -1457,7 +1436,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="2">
         <v>43101</v>
       </c>
@@ -1477,9 +1456,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="2">
-        <v>43101.041666666657</v>
+        <v>43101.04166666666</v>
       </c>
       <c r="B3">
         <v>232.4</v>
@@ -1497,9 +1476,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="2">
-        <v>43101.083333333343</v>
+        <v>43101.08333333334</v>
       </c>
       <c r="B4">
         <v>232.4</v>
@@ -1517,7 +1496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="2">
         <v>43101.125</v>
       </c>
@@ -1537,9 +1516,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="2">
-        <v>43101.166666666657</v>
+        <v>43101.16666666666</v>
       </c>
       <c r="B6">
         <v>232.4</v>
@@ -1557,9 +1536,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="2">
-        <v>43101.208333333343</v>
+        <v>43101.20833333334</v>
       </c>
       <c r="B7">
         <v>232.4</v>
@@ -1577,7 +1556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="2">
         <v>43101.25</v>
       </c>
@@ -1597,9 +1576,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="2">
-        <v>43101.291666666657</v>
+        <v>43101.29166666666</v>
       </c>
       <c r="B9">
         <v>232.4</v>
@@ -1617,9 +1596,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="2">
-        <v>43101.333333333343</v>
+        <v>43101.33333333334</v>
       </c>
       <c r="B10">
         <v>232.4</v>
@@ -1637,7 +1616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="2">
         <v>43101.375</v>
       </c>
@@ -1663,14 +1642,14 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1684,7 +1663,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1707,66 +1686,96 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="B1" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="2">
         <v>43101</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="2">
-        <v>43101.041666666657</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>43101.04166666666</v>
+      </c>
+      <c r="B3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" s="2">
-        <v>43101.083333333343</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>43101.08333333334</v>
+      </c>
+      <c r="B4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" s="2">
         <v>43101.125</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" s="2">
-        <v>43101.166666666657</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>43101.16666666666</v>
+      </c>
+      <c r="B6" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" s="2">
-        <v>43101.208333333343</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>43101.20833333334</v>
+      </c>
+      <c r="B7" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8" s="2">
         <v>43101.25</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9" s="2">
-        <v>43101.291666666657</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>43101.29166666666</v>
+      </c>
+      <c r="B9" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10" s="2">
-        <v>43101.333333333343</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>43101.33333333334</v>
+      </c>
+      <c r="B10" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
       <c r="A11" s="2">
         <v>43101.375</v>
+      </c>
+      <c r="B11" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -1775,14 +1784,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1817,7 +1826,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1855,7 +1864,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1893,7 +1902,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1931,7 +1940,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1969,7 +1978,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -2007,7 +2016,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -2045,7 +2054,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -2083,7 +2092,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -2121,7 +2130,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -2159,7 +2168,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -2197,7 +2206,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -2235,7 +2244,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -2273,7 +2282,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -2311,7 +2320,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -2355,14 +2364,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15">
       <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
@@ -2406,7 +2415,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2432,16 +2441,16 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>1.9380000000000001E-2</v>
+        <v>0.01938</v>
       </c>
       <c r="J2">
-        <v>5.917E-2</v>
+        <v>0.05917</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
       <c r="L2">
-        <v>5.28E-2</v>
+        <v>0.0528</v>
       </c>
       <c r="M2">
         <v>1</v>
@@ -2453,7 +2462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2470,7 +2479,7 @@
         <v>1</v>
       </c>
       <c r="F3">
-        <v>93.949163633082463</v>
+        <v>93.94916363308246</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -2479,16 +2488,16 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <v>5.4030000000000002E-2</v>
+        <v>0.05403</v>
       </c>
       <c r="J3">
-        <v>0.22303999999999999</v>
+        <v>0.22304</v>
       </c>
       <c r="K3">
         <v>0</v>
       </c>
       <c r="L3">
-        <v>4.9200000000000001E-2</v>
+        <v>0.0492</v>
       </c>
       <c r="M3">
         <v>1</v>
@@ -2500,7 +2509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2517,7 +2526,7 @@
         <v>1</v>
       </c>
       <c r="F4">
-        <v>88.909983756153707</v>
+        <v>88.90998375615371</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -2526,16 +2535,16 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <v>4.6989999999999997E-2</v>
+        <v>0.04699</v>
       </c>
       <c r="J4">
-        <v>0.19797000000000001</v>
+        <v>0.19797</v>
       </c>
       <c r="K4">
         <v>0</v>
       </c>
       <c r="L4">
-        <v>4.3799999999999999E-2</v>
+        <v>0.0438</v>
       </c>
       <c r="M4">
         <v>1</v>
@@ -2547,7 +2556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -2564,7 +2573,7 @@
         <v>1</v>
       </c>
       <c r="F5">
-        <v>68.078530509524811</v>
+        <v>68.07853050952481</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -2573,7 +2582,7 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>5.8110000000000002E-2</v>
+        <v>0.05811</v>
       </c>
       <c r="J5">
         <v>0.17632</v>
@@ -2582,7 +2591,7 @@
         <v>0</v>
       </c>
       <c r="L5">
-        <v>3.4000000000000002E-2</v>
+        <v>0.034</v>
       </c>
       <c r="M5">
         <v>1</v>
@@ -2594,7 +2603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -2611,7 +2620,7 @@
         <v>1</v>
       </c>
       <c r="F6">
-        <v>50.753302046046457</v>
+        <v>50.75330204604646</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -2620,16 +2629,16 @@
         <v>0</v>
       </c>
       <c r="I6">
-        <v>5.6950000000000001E-2</v>
+        <v>0.05695</v>
       </c>
       <c r="J6">
-        <v>0.17388000000000001</v>
+        <v>0.17388</v>
       </c>
       <c r="K6">
         <v>0</v>
       </c>
       <c r="L6">
-        <v>3.4599999999999999E-2</v>
+        <v>0.0346</v>
       </c>
       <c r="M6">
         <v>1</v>
@@ -2641,7 +2650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -2658,7 +2667,7 @@
         <v>1</v>
       </c>
       <c r="F7">
-        <v>29.057360099457899</v>
+        <v>29.0573600994579</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -2667,16 +2676,16 @@
         <v>0</v>
       </c>
       <c r="I7">
-        <v>6.701E-2</v>
+        <v>0.06701</v>
       </c>
       <c r="J7">
-        <v>0.17102999999999999</v>
+        <v>0.17103</v>
       </c>
       <c r="K7">
         <v>0</v>
       </c>
       <c r="L7">
-        <v>1.2800000000000001E-2</v>
+        <v>0.0128</v>
       </c>
       <c r="M7">
         <v>1</v>
@@ -2688,7 +2697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -2705,7 +2714,7 @@
         <v>1</v>
       </c>
       <c r="F8">
-        <v>73.720742097279242</v>
+        <v>73.72074209727924</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -2714,10 +2723,10 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <v>1.3350000000000001E-2</v>
+        <v>0.01335</v>
       </c>
       <c r="J8">
-        <v>4.2110000000000002E-2</v>
+        <v>0.04211</v>
       </c>
       <c r="K8">
         <v>0</v>
@@ -2735,7 +2744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -2752,7 +2761,7 @@
         <v>1</v>
       </c>
       <c r="F9">
-        <v>33.677158511309173</v>
+        <v>33.67715851130917</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -2773,7 +2782,7 @@
         <v>0</v>
       </c>
       <c r="M9">
-        <v>0.97799999999999998</v>
+        <v>0.978</v>
       </c>
       <c r="N9">
         <v>0</v>
@@ -2782,7 +2791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -2811,7 +2820,7 @@
         <v>0</v>
       </c>
       <c r="J10">
-        <v>0.55618000000000001</v>
+        <v>0.55618</v>
       </c>
       <c r="K10">
         <v>0</v>
@@ -2820,7 +2829,7 @@
         <v>0</v>
       </c>
       <c r="M10">
-        <v>0.96899999999999997</v>
+        <v>0.969</v>
       </c>
       <c r="N10">
         <v>0</v>
@@ -2829,7 +2838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -2846,7 +2855,7 @@
         <v>1</v>
       </c>
       <c r="F11">
-        <v>58.773265629688908</v>
+        <v>58.77326562968891</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -2858,7 +2867,7 @@
         <v>0</v>
       </c>
       <c r="J11">
-        <v>0.25202000000000002</v>
+        <v>0.25202</v>
       </c>
       <c r="K11">
         <v>0</v>
@@ -2867,7 +2876,7 @@
         <v>0</v>
       </c>
       <c r="M11">
-        <v>0.93200000000000005</v>
+        <v>0.9320000000000001</v>
       </c>
       <c r="N11">
         <v>0</v>
@@ -2876,7 +2885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -2902,10 +2911,10 @@
         <v>0</v>
       </c>
       <c r="I12">
-        <v>9.4979999999999995E-2</v>
+        <v>0.09497999999999999</v>
       </c>
       <c r="J12">
-        <v>0.19889999999999999</v>
+        <v>0.1989</v>
       </c>
       <c r="K12">
         <v>0</v>
@@ -2923,7 +2932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -2940,7 +2949,7 @@
         <v>1</v>
       </c>
       <c r="F13">
-        <v>9.9598084405827105</v>
+        <v>9.959808440582711</v>
       </c>
       <c r="G13">
         <v>0</v>
@@ -2949,10 +2958,10 @@
         <v>0</v>
       </c>
       <c r="I13">
-        <v>0.12291000000000001</v>
+        <v>0.12291</v>
       </c>
       <c r="J13">
-        <v>0.25580999999999998</v>
+        <v>0.25581</v>
       </c>
       <c r="K13">
         <v>0</v>
@@ -2970,7 +2979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -2996,7 +3005,7 @@
         <v>0</v>
       </c>
       <c r="I14">
-        <v>6.615E-2</v>
+        <v>0.06615</v>
       </c>
       <c r="J14">
         <v>0.13027</v>
@@ -3017,7 +3026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -3064,7 +3073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -3081,7 +3090,7 @@
         <v>1</v>
       </c>
       <c r="F16">
-        <v>33.493305704623907</v>
+        <v>33.49330570462391</v>
       </c>
       <c r="G16">
         <v>0</v>
@@ -3111,7 +3120,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -3128,7 +3137,7 @@
         <v>1</v>
       </c>
       <c r="F17">
-        <v>7.1148989032384744</v>
+        <v>7.114898903238474</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -3137,10 +3146,10 @@
         <v>0</v>
       </c>
       <c r="I17">
-        <v>3.1809999999999998E-2</v>
+        <v>0.03181</v>
       </c>
       <c r="J17">
-        <v>8.4500000000000006E-2</v>
+        <v>0.08450000000000001</v>
       </c>
       <c r="K17">
         <v>0</v>
@@ -3158,7 +3167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -3175,7 +3184,7 @@
         <v>1</v>
       </c>
       <c r="F18">
-        <v>11.681277559626411</v>
+        <v>11.68127755962641</v>
       </c>
       <c r="G18">
         <v>0</v>
@@ -3187,7 +3196,7 @@
         <v>0.12711</v>
       </c>
       <c r="J18">
-        <v>0.27038000000000001</v>
+        <v>0.27038</v>
       </c>
       <c r="K18">
         <v>0</v>
@@ -3205,7 +3214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -3222,7 +3231,7 @@
         <v>1</v>
       </c>
       <c r="F19">
-        <v>5.8311900127158669</v>
+        <v>5.831190012715867</v>
       </c>
       <c r="G19">
         <v>0</v>
@@ -3231,10 +3240,10 @@
         <v>0</v>
       </c>
       <c r="I19">
-        <v>8.2049999999999998E-2</v>
+        <v>0.08205</v>
       </c>
       <c r="J19">
-        <v>0.19206999999999999</v>
+        <v>0.19207</v>
       </c>
       <c r="K19">
         <v>0</v>
@@ -3252,7 +3261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -3278,7 +3287,7 @@
         <v>0</v>
       </c>
       <c r="I20">
-        <v>0.22092000000000001</v>
+        <v>0.22092</v>
       </c>
       <c r="J20">
         <v>0.19988</v>
@@ -3299,7 +3308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -3316,7 +3325,7 @@
         <v>1</v>
       </c>
       <c r="F21">
-        <v>7.5869852716979551</v>
+        <v>7.586985271697955</v>
       </c>
       <c r="G21">
         <v>0</v>
@@ -3352,16 +3361,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
@@ -3381,7 +3388,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3404,7 +3411,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3427,7 +3434,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -3450,7 +3457,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -3473,7 +3480,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -3496,7 +3503,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -3519,7 +3526,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -3542,7 +3549,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -3565,7 +3572,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -3588,7 +3595,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -3611,7 +3618,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -3640,23 +3647,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:L18"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.5703125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="B1" s="1" t="s">
         <v>128</v>
       </c>
@@ -3691,7 +3689,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2" s="2">
         <v>43101</v>
       </c>
@@ -3729,9 +3727,9 @@
         <v>149</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3" s="2">
-        <v>43101.041666666657</v>
+        <v>43101.04166666666</v>
       </c>
       <c r="B3" t="s">
         <v>139</v>
@@ -3767,9 +3765,9 @@
         <v>149</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4" s="2">
-        <v>43101.083333333343</v>
+        <v>43101.08333333334</v>
       </c>
       <c r="B4" t="s">
         <v>139</v>
@@ -3805,7 +3803,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="A5" s="2">
         <v>43101.125</v>
       </c>
@@ -3843,9 +3841,9 @@
         <v>149</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12">
       <c r="A6" s="2">
-        <v>43101.166666666657</v>
+        <v>43101.16666666666</v>
       </c>
       <c r="B6" t="s">
         <v>139</v>
@@ -3881,9 +3879,9 @@
         <v>149</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12">
       <c r="A7" s="2">
-        <v>43101.208333333343</v>
+        <v>43101.20833333334</v>
       </c>
       <c r="B7" t="s">
         <v>139</v>
@@ -3919,7 +3917,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12">
       <c r="A8" s="2">
         <v>43101.25</v>
       </c>
@@ -3957,9 +3955,9 @@
         <v>149</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12">
       <c r="A9" s="2">
-        <v>43101.291666666657</v>
+        <v>43101.29166666666</v>
       </c>
       <c r="B9" t="s">
         <v>139</v>
@@ -3995,9 +3993,9 @@
         <v>149</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12">
       <c r="A10" s="2">
-        <v>43101.333333333343</v>
+        <v>43101.33333333334</v>
       </c>
       <c r="B10" t="s">
         <v>139</v>
@@ -4033,7 +4031,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12">
       <c r="A11" s="2">
         <v>43101.375</v>
       </c>
@@ -4077,14 +4075,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="B1" s="1" t="s">
         <v>128</v>
       </c>
@@ -4119,7 +4117,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2" s="2">
         <v>43101</v>
       </c>
@@ -4157,9 +4155,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3" s="2">
-        <v>43101.041666666657</v>
+        <v>43101.04166666666</v>
       </c>
       <c r="B3" t="s">
         <v>48</v>
@@ -4195,9 +4193,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4" s="2">
-        <v>43101.083333333343</v>
+        <v>43101.08333333334</v>
       </c>
       <c r="B4" t="s">
         <v>48</v>
@@ -4233,7 +4231,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="A5" s="2">
         <v>43101.125</v>
       </c>
@@ -4271,9 +4269,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12">
       <c r="A6" s="2">
-        <v>43101.166666666657</v>
+        <v>43101.16666666666</v>
       </c>
       <c r="B6" t="s">
         <v>48</v>
@@ -4309,9 +4307,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12">
       <c r="A7" s="2">
-        <v>43101.208333333343</v>
+        <v>43101.20833333334</v>
       </c>
       <c r="B7" t="s">
         <v>48</v>
@@ -4347,7 +4345,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12">
       <c r="A8" s="2">
         <v>43101.25</v>
       </c>
@@ -4385,9 +4383,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12">
       <c r="A9" s="2">
-        <v>43101.291666666657</v>
+        <v>43101.29166666666</v>
       </c>
       <c r="B9" t="s">
         <v>48</v>
@@ -4423,9 +4421,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12">
       <c r="A10" s="2">
-        <v>43101.333333333343</v>
+        <v>43101.33333333334</v>
       </c>
       <c r="B10" t="s">
         <v>48</v>
@@ -4461,7 +4459,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12">
       <c r="A11" s="2">
         <v>43101.375</v>
       </c>
@@ -4505,14 +4503,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="B1" s="1" t="s">
         <v>128</v>
       </c>
@@ -4547,7 +4545,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2" s="2">
         <v>43101</v>
       </c>
@@ -4585,9 +4583,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3" s="2">
-        <v>43101.041666666657</v>
+        <v>43101.04166666666</v>
       </c>
       <c r="B3" t="s">
         <v>48</v>
@@ -4623,9 +4621,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4" s="2">
-        <v>43101.083333333343</v>
+        <v>43101.08333333334</v>
       </c>
       <c r="B4" t="s">
         <v>48</v>
@@ -4661,7 +4659,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="A5" s="2">
         <v>43101.125</v>
       </c>
@@ -4699,9 +4697,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12">
       <c r="A6" s="2">
-        <v>43101.166666666657</v>
+        <v>43101.16666666666</v>
       </c>
       <c r="B6" t="s">
         <v>48</v>
@@ -4737,9 +4735,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12">
       <c r="A7" s="2">
-        <v>43101.208333333343</v>
+        <v>43101.20833333334</v>
       </c>
       <c r="B7" t="s">
         <v>48</v>
@@ -4775,7 +4773,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12">
       <c r="A8" s="2">
         <v>43101.25</v>
       </c>
@@ -4813,9 +4811,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12">
       <c r="A9" s="2">
-        <v>43101.291666666657</v>
+        <v>43101.29166666666</v>
       </c>
       <c r="B9" t="s">
         <v>48</v>
@@ -4851,9 +4849,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12">
       <c r="A10" s="2">
-        <v>43101.333333333343</v>
+        <v>43101.33333333334</v>
       </c>
       <c r="B10" t="s">
         <v>48</v>
@@ -4889,7 +4887,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12">
       <c r="A11" s="2">
         <v>43101.375</v>
       </c>
@@ -4933,14 +4931,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:5">
       <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
@@ -4960,14 +4958,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:10">
       <c r="B1" s="1" t="s">
         <v>6</v>
       </c>

</xml_diff>